<commit_message>
Fix model adapt to the new Bang Bao Gia 2016 specs, integrate phuongphapphantich into chitieuphantich as a field, nhomphantich has it one to many relationship with chitieuphantich
</commit_message>
<xml_diff>
--- a/Documents/ChiTieuPhanTich-ExcelSheet/chitieupt-samplesheet.xlsx
+++ b/Documents/ChiTieuPhanTich-ExcelSheet/chitieupt-samplesheet.xlsx
@@ -31,10 +31,10 @@
     <t xml:space="preserve">Tên Chỉ Tiêu</t>
   </si>
   <si>
+    <t xml:space="preserve">Phương Pháp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Đơn Giá</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phương Pháp</t>
   </si>
   <si>
     <t xml:space="preserve">Nước</t>
@@ -205,6 +205,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -459,13 +460,14 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.04"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.22"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -498,20 +500,20 @@
       <c r="B3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="0" t="s">
+      <c r="C5" s="0" t="s">
         <v>9</v>
       </c>
     </row>
@@ -519,15 +521,15 @@
       <c r="B6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="0" t="n">
         <v>10000</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="0" t="s">
+      <c r="C7" s="0" t="s">
         <v>12</v>
       </c>
     </row>
@@ -538,15 +540,15 @@
       <c r="B8" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="0" t="n">
         <v>1000000</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="0" t="s">
+      <c r="C9" s="0" t="s">
         <v>16</v>
       </c>
     </row>
@@ -554,11 +556,11 @@
       <c r="B10" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="0" t="n">
         <v>30000</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -568,15 +570,15 @@
       <c r="B11" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="0" t="n">
         <v>20001</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D12" s="0" t="s">
+      <c r="C12" s="0" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finish first iteration of SoNhanMau task
</commit_message>
<xml_diff>
--- a/Documents/ChiTieuPhanTich-ExcelSheet/chitieupt-samplesheet.xlsx
+++ b/Documents/ChiTieuPhanTich-ExcelSheet/chitieupt-samplesheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t xml:space="preserve">CHỈ TIÊU PHÂN TÍCH</t>
   </si>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Đơn Giá</t>
   </si>
   <si>
-    <t xml:space="preserve">Nước</t>
+    <t xml:space="preserve">Nước Thải</t>
   </si>
   <si>
     <t xml:space="preserve">abc</t>
@@ -46,9 +46,15 @@
     <t xml:space="preserve">PP1</t>
   </si>
   <si>
+    <t xml:space="preserve">abc1</t>
+  </si>
+  <si>
     <t xml:space="preserve">PP2</t>
   </si>
   <si>
+    <t xml:space="preserve">sss</t>
+  </si>
+  <si>
     <t xml:space="preserve">PP3</t>
   </si>
   <si>
@@ -58,6 +64,9 @@
     <t xml:space="preserve">PPACC1</t>
   </si>
   <si>
+    <t xml:space="preserve">kiss</t>
+  </si>
+  <si>
     <t xml:space="preserve">PPACC2</t>
   </si>
   <si>
@@ -68,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">BTPP0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ds</t>
   </si>
   <si>
     <t xml:space="preserve">BTPP11</t>
@@ -460,7 +472,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -508,56 +520,80 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>8</v>
+      </c>
       <c r="C4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>2222</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>10</v>
+      </c>
       <c r="C5" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>10000</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>14</v>
+      </c>
       <c r="C7" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1000000</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="C9" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>222</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>30000</v>
@@ -565,21 +601,27 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>20001</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>24</v>
+      </c>
       <c r="C12" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>2222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalize demo for 9/3/2017
</commit_message>
<xml_diff>
--- a/Documents/ChiTieuPhanTich-ExcelSheet/chitieupt-samplesheet.xlsx
+++ b/Documents/ChiTieuPhanTich-ExcelSheet/chitieupt-samplesheet.xlsx
@@ -139,6 +139,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -169,6 +170,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -189,6 +191,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -219,6 +222,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -243,6 +247,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">4</t>
     </r>
@@ -253,6 +258,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2-</t>
     </r>
@@ -282,6 +288,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">4</t>
     </r>
@@ -291,6 +298,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2-</t>
     </r>
@@ -327,6 +335,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">4</t>
     </r>
@@ -337,6 +346,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3-</t>
     </r>
@@ -367,6 +377,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3</t>
     </r>
@@ -377,6 +388,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -401,6 +413,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -411,6 +424,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -431,6 +445,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -440,6 +455,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -470,6 +486,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3 tự do</t>
     </r>
@@ -490,6 +507,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3</t>
     </r>
@@ -537,6 +555,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2-</t>
     </r>
@@ -567,6 +586,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3</t>
     </r>
@@ -577,6 +597,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2-</t>
     </r>
@@ -607,6 +628,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">5</t>
     </r>
@@ -641,6 +663,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">  5540 : 2012</t>
     </r>
@@ -673,6 +696,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">+6</t>
     </r>
@@ -705,6 +729,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">+3</t>
     </r>
@@ -801,6 +826,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -886,6 +912,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">  2012 – 9215 C</t>
     </r>
@@ -967,6 +994,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -1015,6 +1043,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">s</t>
     </r>
@@ -1045,6 +1074,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -1074,6 +1104,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -1104,6 +1135,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">s </t>
     </r>
@@ -1131,6 +1163,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2 </t>
     </r>
@@ -1164,6 +1197,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -1271,6 +1305,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">00000</t>
     </r>
@@ -1342,10 +1377,10 @@
     <t xml:space="preserve">24 - D</t>
   </si>
   <si>
-    <t xml:space="preserve">12 -  Dicloropropan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 -  Dichloropropen</t>
+    <t xml:space="preserve">12 – Dicloropropan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 – Dichloropropen</t>
   </si>
   <si>
     <t xml:space="preserve">Heptaclo và heptaclo epoxit</t>
@@ -1429,6 +1464,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Dibromoclorometan</t>
     </r>
@@ -1464,6 +1500,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Xyano clorit (tính theo C</t>
     </r>
@@ -1482,6 +1519,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -1530,6 +1568,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -1584,6 +1623,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -1638,6 +1678,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">6+)</t>
     </r>
@@ -1691,6 +1732,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -1799,6 +1841,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -1832,6 +1875,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -1851,6 +1895,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">5</t>
     </r>
@@ -1896,6 +1941,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">s</t>
     </r>
@@ -1982,6 +2028,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(#)</t>
     </r>
@@ -2031,6 +2078,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">+</t>
     </r>
@@ -2121,6 +2169,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -2154,6 +2203,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3</t>
     </r>
@@ -2168,6 +2218,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">NO</t>
     </r>
@@ -2178,6 +2229,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -2192,6 +2244,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">SO</t>
     </r>
@@ -2202,6 +2255,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -2232,6 +2286,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -2256,6 +2311,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3</t>
     </r>
@@ -2325,6 +2381,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">4</t>
     </r>
@@ -2366,6 +2423,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -2384,6 +2442,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -2419,7 +2478,7 @@
     <t xml:space="preserve">Không Khí Tại Nguồn</t>
   </si>
   <si>
-    <t xml:space="preserve">Khí thải lò đốt  lò hơi</t>
+    <t xml:space="preserve">Khí thải  lò đốt lò hơi</t>
   </si>
   <si>
     <t xml:space="preserve">Thiết bị chuyên dụng Testto 350 XL</t>
@@ -2434,6 +2493,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">NO</t>
     </r>
@@ -2444,6 +2504,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">x</t>
     </r>
@@ -2455,6 +2516,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CO</t>
     </r>
@@ -2465,6 +2527,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -2479,6 +2542,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">O</t>
     </r>
@@ -2489,6 +2553,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -2509,6 +2574,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">NH</t>
     </r>
@@ -2519,6 +2585,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3</t>
     </r>
@@ -2533,6 +2600,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">H</t>
     </r>
@@ -2543,6 +2611,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -2552,6 +2621,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">S</t>
     </r>
@@ -2563,6 +2633,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">T</t>
     </r>
@@ -2592,6 +2663,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3</t>
     </r>
@@ -2612,6 +2684,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -2630,6 +2703,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">4 </t>
     </r>
@@ -2648,6 +2722,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3</t>
     </r>
@@ -2677,6 +2752,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">4</t>
     </r>
@@ -2698,7 +2774,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2826,6 +2902,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
@@ -2833,6 +2910,7 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <vertAlign val="subscript"/>
@@ -2840,23 +2918,21 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <vertAlign val="subscript"/>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -3089,7 +3165,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3145,7 +3221,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3244,15 +3320,15 @@
   </sheetPr>
   <dimension ref="A1:D434"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A418" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C425" activeCellId="0" sqref="C425"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A382" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B393" activeCellId="0" sqref="B393"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.22"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>

</xml_diff>